<commit_message>
changes from Friday. progress table and synapsida marg rates issue
</commit_message>
<xml_diff>
--- a/analyses_log.xlsx
+++ b/analyses_log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\BDNN_Arielli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoesLabAdmin\Documents\BDNN_Arielli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F99CE426-57FB-4A01-9014-693AA1AEC635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0637504D-DCFF-4624-AA26-9E5E0B2FB6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
+    <workbookView xWindow="840" yWindow="729" windowWidth="23091" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="2" r:id="rId1"/>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EA881A-93D2-4F0C-B578-B509C4BBF0BD}">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.4"/>
@@ -1435,8 +1435,8 @@
       <c r="M15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="N15" s="4" t="s">
-        <v>15</v>
+      <c r="N15" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="O15" s="4" t="s">
         <v>15</v>
@@ -1821,8 +1821,8 @@
       <c r="M22" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="N22" s="4" t="s">
-        <v>15</v>
+      <c r="N22" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="O22" s="4" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
pulled B_bdnn restored for tem from cluster, update to progress log
</commit_message>
<xml_diff>
--- a/analyses_log.xlsx
+++ b/analyses_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoesLabAdmin\Documents\BDNN_Arielli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0637504D-DCFF-4624-AA26-9E5E0B2FB6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59A9633-B5F2-4EE8-BEC8-147D7A0F082B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="729" windowWidth="23091" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
+    <workbookView xWindow="-189" yWindow="934" windowWidth="23092" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="2" r:id="rId1"/>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EA881A-93D2-4F0C-B578-B509C4BBF0BD}">
   <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.4"/>
@@ -1114,8 +1114,8 @@
       <c r="N9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O9" s="4" t="s">
-        <v>15</v>
+      <c r="O9" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>12</v>
@@ -1170,8 +1170,8 @@
       <c r="N10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="4" t="s">
-        <v>15</v>
+      <c r="O10" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
A_mcmc scripts, B_covar renamed to B_covar_rjmcmc, edits to progress log
</commit_message>
<xml_diff>
--- a/analyses_log.xlsx
+++ b/analyses_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoesLabAdmin\Documents\BDNN_Arielli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59A9633-B5F2-4EE8-BEC8-147D7A0F082B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C382C5C8-3587-4D4B-8609-1A33F850F2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-189" yWindow="934" windowWidth="23092" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
+    <workbookView xWindow="283" yWindow="1774" windowWidth="27111" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="62">
   <si>
     <t>Sampling Algorithm</t>
   </si>
@@ -221,6 +221,18 @@
   </si>
   <si>
     <t>Age Sampling Replicates</t>
+  </si>
+  <si>
+    <t>MCMC</t>
+  </si>
+  <si>
+    <t>Compare with 1 Myr RJMCMC, no preds</t>
+  </si>
+  <si>
+    <t>Compare with 1 Myr BDMCMC, no preds, and CoVar RJMCMC</t>
+  </si>
+  <si>
+    <t>CoVa + MBD</t>
   </si>
 </sst>
 </file>
@@ -673,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EA881A-93D2-4F0C-B578-B509C4BBF0BD}">
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.4"/>
@@ -697,7 +709,7 @@
     <col min="15" max="15" width="13.07421875" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.84375" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="13.07421875" style="3" customWidth="1"/>
-    <col min="18" max="18" width="35.3046875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="48.15234375" style="3" customWidth="1"/>
     <col min="19" max="16384" width="9.23046875" style="3"/>
   </cols>
   <sheetData>
@@ -757,38 +769,72 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="E2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="3">
+        <v>10</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="S2" s="3"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A3" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>48</v>
@@ -832,213 +878,130 @@
       <c r="Q3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A4" s="7" t="s">
+      <c r="R3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="3">
+        <v>10</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="3">
-        <v>10</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="S4" s="2"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="C7" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="3" t="s">
+      <c r="E7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="3">
-        <v>10</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="3">
-        <v>10</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>15</v>
+      <c r="G7" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A8" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>11</v>
@@ -1046,8 +1009,8 @@
       <c r="J8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>56</v>
+      <c r="K8" s="3">
+        <v>10</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>34</v>
@@ -1065,10 +1028,7 @@
         <v>12</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
@@ -1079,13 +1039,13 @@
         <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>27</v>
@@ -1121,7 +1081,7 @@
         <v>12</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="R9" s="3" t="s">
         <v>29</v>
@@ -1135,13 +1095,13 @@
         <v>32</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>27</v>
@@ -1185,25 +1145,25 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A11" s="7" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>39</v>
@@ -1214,8 +1174,8 @@
       <c r="J11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="3">
-        <v>10</v>
+      <c r="K11" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>34</v>
@@ -1235,58 +1195,25 @@
       <c r="Q11" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K12" s="3">
-        <v>10</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>15</v>
+      <c r="R11" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.4">
@@ -1297,7 +1224,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>9</v>
@@ -1305,14 +1232,14 @@
       <c r="E13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>51</v>
+      <c r="F13" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>11</v>
@@ -1350,7 +1277,7 @@
         <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>9</v>
@@ -1365,7 +1292,7 @@
         <v>51</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>11</v>
@@ -1403,7 +1330,7 @@
         <v>32</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>9</v>
@@ -1412,13 +1339,13 @@
         <v>40</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>11</v>
@@ -1438,8 +1365,8 @@
       <c r="N15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O15" s="4" t="s">
-        <v>15</v>
+      <c r="O15" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="P15" s="3" t="s">
         <v>12</v>
@@ -1456,7 +1383,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>9</v>
@@ -1465,13 +1392,13 @@
         <v>40</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>11</v>
@@ -1506,10 +1433,10 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>9</v>
@@ -1518,13 +1445,13 @@
         <v>40</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>11</v>
@@ -1544,8 +1471,8 @@
       <c r="N17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O17" s="3" t="s">
-        <v>14</v>
+      <c r="O17" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>12</v>
@@ -1553,19 +1480,16 @@
       <c r="Q17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R17" s="3" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A18" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>9</v>
@@ -1574,13 +1498,13 @@
         <v>40</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>11</v>
@@ -1600,8 +1524,8 @@
       <c r="N18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O18" s="4" t="s">
-        <v>22</v>
+      <c r="O18" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="P18" s="3" t="s">
         <v>12</v>
@@ -1609,9 +1533,6 @@
       <c r="Q18" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R18" s="3" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
@@ -1621,7 +1542,7 @@
         <v>31</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>9</v>
@@ -1630,13 +1551,13 @@
         <v>40</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>11</v>
@@ -1656,8 +1577,8 @@
       <c r="N19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O19" s="4" t="s">
-        <v>22</v>
+      <c r="O19" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>12</v>
@@ -1677,7 +1598,7 @@
         <v>31</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>9</v>
@@ -1692,7 +1613,7 @@
         <v>52</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>11</v>
@@ -1733,7 +1654,7 @@
         <v>31</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>9</v>
@@ -1748,7 +1669,7 @@
         <v>52</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>11</v>
@@ -1789,7 +1710,7 @@
         <v>31</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>9</v>
@@ -1798,13 +1719,13 @@
         <v>40</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>11</v>
@@ -1825,12 +1746,124 @@
         <v>14</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="P22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="Q22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" s="3">
+        <v>10</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24" s="3">
+        <v>10</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q24" s="3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EOD tuesday progress log
</commit_message>
<xml_diff>
--- a/analyses_log.xlsx
+++ b/analyses_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoesLabAdmin\Documents\BDNN_Arielli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{762B8CCA-5D07-485E-87D7-222F722066B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF6D6CF-CEEC-43C3-8510-59C3B3ECF2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="283" yWindow="1774" windowWidth="27111" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="66">
   <si>
     <t>Sampling Algorithm</t>
   </si>
@@ -190,9 +190,6 @@
     <t>Original</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>no predictor</t>
   </si>
   <si>
@@ -217,9 +214,6 @@
     <t>Time + Diversity</t>
   </si>
   <si>
-    <t>9*</t>
-  </si>
-  <si>
     <t>Age Sampling Replicates</t>
   </si>
   <si>
@@ -239,6 +233,18 @@
   </si>
   <si>
     <t>102 mi</t>
+  </si>
+  <si>
+    <t>103 mi</t>
+  </si>
+  <si>
+    <t>104 mi</t>
+  </si>
+  <si>
+    <t>105 mi</t>
+  </si>
+  <si>
+    <t>106 mi</t>
   </si>
 </sst>
 </file>
@@ -275,7 +281,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,12 +297,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,11 +336,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -355,6 +352,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -700,7 +700,7 @@
   <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.4"/>
@@ -736,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>45</v>
@@ -745,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>44</v>
@@ -757,7 +757,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>4</v>
@@ -792,7 +792,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>40</v>
@@ -834,7 +834,7 @@
         <v>14</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S2" s="3"/>
     </row>
@@ -849,7 +849,7 @@
         <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>40</v>
@@ -891,19 +891,19 @@
         <v>14</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="S3" s="2"/>
     </row>
     <row r="4" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>32</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>40</v>
@@ -927,7 +927,7 @@
         <v>11</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>33</v>
@@ -935,19 +935,25 @@
       <c r="N4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="O4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>40</v>
@@ -971,7 +977,7 @@
         <v>12</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>33</v>
@@ -979,7 +985,13 @@
       <c r="N5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1036,24 +1048,48 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="E7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>40</v>
+      <c r="G7" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="8">
+        <v>11</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
@@ -1064,7 +1100,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>18</v>
@@ -1088,10 +1124,10 @@
         <v>13</v>
       </c>
       <c r="K8" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>33</v>
@@ -1117,7 +1153,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>19</v>
@@ -1129,7 +1165,7 @@
         <v>27</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>39</v>
@@ -1140,11 +1176,11 @@
       <c r="J9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>56</v>
+      <c r="K9" s="3">
+        <v>13</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>33</v>
@@ -1173,7 +1209,7 @@
         <v>32</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>19</v>
@@ -1185,7 +1221,7 @@
         <v>27</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>39</v>
@@ -1196,11 +1232,11 @@
       <c r="J10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>56</v>
+      <c r="K10" s="3">
+        <v>14</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>34</v>
+        <v>63</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>33</v>
@@ -1229,7 +1265,7 @@
         <v>32</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>19</v>
@@ -1241,7 +1277,7 @@
         <v>27</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>39</v>
@@ -1252,11 +1288,11 @@
       <c r="J11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>56</v>
+      <c r="K11" s="3">
+        <v>15</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>33</v>
@@ -1277,21 +1313,51 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="10" t="s">
+    <row r="12" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="9" t="s">
+      <c r="C12" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="8" t="s">
         <v>42</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K12" s="8">
+        <v>16</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.4">
@@ -1302,7 +1368,7 @@
         <v>32</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>9</v>
@@ -1310,11 +1376,11 @@
       <c r="E13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>40</v>
+      <c r="F13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>39</v>
@@ -1355,7 +1421,7 @@
         <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>9</v>
@@ -1364,10 +1430,10 @@
         <v>40</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>37</v>
@@ -1408,7 +1474,7 @@
         <v>32</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>9</v>
@@ -1417,10 +1483,10 @@
         <v>40</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>28</v>
@@ -1461,7 +1527,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>9</v>
@@ -1470,10 +1536,10 @@
         <v>40</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>26</v>
@@ -1514,7 +1580,7 @@
         <v>32</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>9</v>
@@ -1523,7 +1589,7 @@
         <v>40</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>40</v>
@@ -1567,7 +1633,7 @@
         <v>32</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>9</v>
@@ -1576,7 +1642,7 @@
         <v>40</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>40</v>
@@ -1620,7 +1686,7 @@
         <v>31</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>9</v>
@@ -1629,7 +1695,7 @@
         <v>40</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>40</v>
@@ -1676,7 +1742,7 @@
         <v>31</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>9</v>
@@ -1685,10 +1751,10 @@
         <v>40</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>35</v>
@@ -1732,7 +1798,7 @@
         <v>31</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>9</v>
@@ -1741,10 +1807,10 @@
         <v>40</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>36</v>
@@ -1788,7 +1854,7 @@
         <v>31</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>9</v>
@@ -1797,10 +1863,10 @@
         <v>40</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>37</v>
@@ -1844,7 +1910,7 @@
         <v>31</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>9</v>
@@ -1853,10 +1919,10 @@
         <v>40</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>38</v>
@@ -1900,7 +1966,7 @@
         <v>31</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>9</v>
@@ -1909,7 +1975,7 @@
         <v>40</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
B_covar_mcmc scripts, update to log reflecting that
</commit_message>
<xml_diff>
--- a/analyses_log.xlsx
+++ b/analyses_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoesLabAdmin\Documents\BDNN_Arielli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF6D6CF-CEEC-43C3-8510-59C3B3ECF2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F39E905-2B73-4FFA-81A1-BF51CC1378AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="283" yWindow="1774" windowWidth="27111" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
+    <workbookView xWindow="1543" yWindow="1311" windowWidth="27111" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="59">
   <si>
     <t>Sampling Algorithm</t>
   </si>
@@ -224,27 +224,6 @@
   </si>
   <si>
     <t>Compare with 1 Myr BDMCMC, no preds, and CoVar RJMCMC</t>
-  </si>
-  <si>
-    <t>CoVa + MBD</t>
-  </si>
-  <si>
-    <t>101 mi</t>
-  </si>
-  <si>
-    <t>102 mi</t>
-  </si>
-  <si>
-    <t>103 mi</t>
-  </si>
-  <si>
-    <t>104 mi</t>
-  </si>
-  <si>
-    <t>105 mi</t>
-  </si>
-  <si>
-    <t>106 mi</t>
   </si>
 </sst>
 </file>
@@ -697,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EA881A-93D2-4F0C-B578-B509C4BBF0BD}">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.4"/>
@@ -923,11 +902,11 @@
       <c r="J4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="2">
-        <v>11</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>60</v>
+      <c r="K4" s="3">
+        <v>10</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>33</v>
@@ -974,10 +953,10 @@
         <v>13</v>
       </c>
       <c r="K5" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>33</v>
@@ -1048,47 +1027,53 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="9" t="s">
+    <row r="7" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="8" t="s">
+      <c r="E7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="8">
-        <v>11</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q7" s="8" t="s">
+      <c r="G7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="2">
+        <v>10</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1124,10 +1109,10 @@
         <v>13</v>
       </c>
       <c r="K8" s="3">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>33</v>
@@ -1177,10 +1162,10 @@
         <v>13</v>
       </c>
       <c r="K9" s="3">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>33</v>
@@ -1233,10 +1218,10 @@
         <v>13</v>
       </c>
       <c r="K10" s="3">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>33</v>
@@ -1289,10 +1274,10 @@
         <v>13</v>
       </c>
       <c r="K11" s="3">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>33</v>
@@ -1315,7 +1300,7 @@
     </row>
     <row r="12" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="8" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>31</v>
@@ -1342,10 +1327,10 @@
         <v>13</v>
       </c>
       <c r="K12" s="8">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="M12" s="8" t="s">
         <v>33</v>
@@ -1360,56 +1345,50 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="3" t="s">
+    <row r="13" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="3" t="s">
+      <c r="D13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="3">
-        <v>10</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O13" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q13" s="3" t="s">
+      <c r="I13" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="8">
+        <v>10</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q13" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1436,7 +1415,7 @@
         <v>50</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>11</v>
@@ -1489,7 +1468,7 @@
         <v>50</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>11</v>
@@ -1542,7 +1521,7 @@
         <v>50</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>11</v>
@@ -1589,13 +1568,13 @@
         <v>40</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>11</v>
@@ -1615,8 +1594,8 @@
       <c r="N17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O17" s="4" t="s">
-        <v>15</v>
+      <c r="O17" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="P17" s="3" t="s">
         <v>12</v>
@@ -1642,13 +1621,13 @@
         <v>40</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>40</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>11</v>
@@ -1668,8 +1647,8 @@
       <c r="N18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O18" s="3" t="s">
-        <v>14</v>
+      <c r="O18" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="P18" s="3" t="s">
         <v>12</v>
@@ -1683,7 +1662,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>56</v>
@@ -1730,9 +1709,6 @@
       <c r="Q19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R19" s="3" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A20" s="7" t="s">
@@ -1751,13 +1727,13 @@
         <v>40</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>11</v>
@@ -1777,8 +1753,8 @@
       <c r="N20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O20" s="4" t="s">
-        <v>22</v>
+      <c r="O20" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="P20" s="3" t="s">
         <v>12</v>
@@ -1813,7 +1789,7 @@
         <v>51</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>11</v>
@@ -1869,7 +1845,7 @@
         <v>51</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>11</v>
@@ -1925,7 +1901,7 @@
         <v>51</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>11</v>
@@ -1975,39 +1951,95 @@
         <v>40</v>
       </c>
       <c r="F24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K24" s="3">
+        <v>10</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K24" s="3">
-        <v>10</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="O24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="P24" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q24" s="3" t="s">
+      <c r="G25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K25" s="3">
+        <v>10</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q25" s="3" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
hespdiv binned data fully run, plus B_bdnn_rep scripts from cluster
</commit_message>
<xml_diff>
--- a/analyses_log.xlsx
+++ b/analyses_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoesLabAdmin\Documents\BDNN_Arielli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F39E905-2B73-4FFA-81A1-BF51CC1378AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AB471A-9C16-422E-8C56-95E3DA3DD86F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1543" yWindow="1311" windowWidth="27111" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
+    <workbookView xWindow="334" yWindow="1671" windowWidth="31997" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="2" r:id="rId1"/>
@@ -115,9 +115,6 @@
     <t>CoVar RJMCMC</t>
   </si>
   <si>
-    <t>Tem Only</t>
-  </si>
-  <si>
     <t>Graphed?</t>
   </si>
   <si>
@@ -224,6 +221,9 @@
   </si>
   <si>
     <t>Compare with 1 Myr BDMCMC, no preds, and CoVar RJMCMC</t>
+  </si>
+  <si>
+    <t>Syn No</t>
   </si>
 </sst>
 </file>
@@ -679,7 +679,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.4"/>
@@ -706,28 +706,28 @@
   <sheetData>
     <row r="1" spans="1:19" s="5" customFormat="1" ht="25.75" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>2</v>
@@ -736,7 +736,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>4</v>
@@ -754,10 +754,10 @@
         <v>8</v>
       </c>
       <c r="Q1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
@@ -765,22 +765,22 @@
         <v>17</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>10</v>
@@ -795,10 +795,10 @@
         <v>10</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>14</v>
@@ -813,7 +813,7 @@
         <v>14</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="S2" s="3"/>
     </row>
@@ -822,22 +822,22 @@
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>10</v>
@@ -852,10 +852,10 @@
         <v>10</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>14</v>
@@ -870,28 +870,28 @@
         <v>14</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S3" s="2"/>
     </row>
     <row r="4" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>10</v>
@@ -906,10 +906,10 @@
         <v>10</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>14</v>
@@ -926,22 +926,22 @@
     </row>
     <row r="5" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B5" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>10</v>
@@ -956,10 +956,10 @@
         <v>10</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N5" s="2" t="s">
         <v>14</v>
@@ -979,7 +979,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>16</v>
@@ -988,16 +988,16 @@
         <v>18</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>11</v>
@@ -1009,10 +1009,10 @@
         <v>10</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>14</v>
@@ -1032,22 +1032,22 @@
         <v>18</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>11</v>
@@ -1059,10 +1059,10 @@
         <v>10</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N7" s="2" t="s">
         <v>14</v>
@@ -1082,25 +1082,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>11</v>
@@ -1112,10 +1112,10 @@
         <v>10</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N8" s="3" t="s">
         <v>14</v>
@@ -1135,25 +1135,25 @@
         <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>11</v>
@@ -1165,10 +1165,10 @@
         <v>10</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N9" s="3" t="s">
         <v>14</v>
@@ -1183,7 +1183,7 @@
         <v>14</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.4">
@@ -1191,25 +1191,25 @@
         <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>11</v>
@@ -1221,10 +1221,10 @@
         <v>10</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N10" s="3" t="s">
         <v>14</v>
@@ -1239,7 +1239,7 @@
         <v>15</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.4">
@@ -1247,25 +1247,25 @@
         <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>11</v>
@@ -1277,10 +1277,10 @@
         <v>10</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N11" s="3" t="s">
         <v>14</v>
@@ -1295,7 +1295,7 @@
         <v>15</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.4">
@@ -1303,22 +1303,22 @@
         <v>19</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>11</v>
@@ -1330,10 +1330,10 @@
         <v>10</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N12" s="12" t="s">
         <v>15</v>
@@ -1350,22 +1350,22 @@
         <v>19</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="8" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I13" s="8" t="s">
         <v>11</v>
@@ -1377,10 +1377,10 @@
         <v>10</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N13" s="12" t="s">
         <v>15</v>
@@ -1397,25 +1397,25 @@
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>11</v>
@@ -1427,10 +1427,10 @@
         <v>10</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N14" s="3" t="s">
         <v>14</v>
@@ -1450,25 +1450,25 @@
         <v>9</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>11</v>
@@ -1480,10 +1480,10 @@
         <v>10</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N15" s="3" t="s">
         <v>14</v>
@@ -1503,25 +1503,25 @@
         <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>11</v>
@@ -1533,10 +1533,10 @@
         <v>10</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>14</v>
@@ -1556,25 +1556,25 @@
         <v>9</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I17" s="3" t="s">
         <v>11</v>
@@ -1586,10 +1586,10 @@
         <v>10</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N17" s="3" t="s">
         <v>14</v>
@@ -1609,25 +1609,25 @@
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>11</v>
@@ -1639,10 +1639,10 @@
         <v>10</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>14</v>
@@ -1662,22 +1662,22 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>10</v>
@@ -1692,10 +1692,10 @@
         <v>10</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N19" s="3" t="s">
         <v>14</v>
@@ -1715,22 +1715,22 @@
         <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>10</v>
@@ -1745,10 +1745,10 @@
         <v>10</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>14</v>
@@ -1763,7 +1763,7 @@
         <v>15</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.4">
@@ -1771,25 +1771,25 @@
         <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>11</v>
@@ -1801,16 +1801,16 @@
         <v>10</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N21" s="3" t="s">
         <v>14</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="P21" s="3" t="s">
         <v>12</v>
@@ -1819,7 +1819,7 @@
         <v>15</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.4">
@@ -1827,25 +1827,25 @@
         <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>11</v>
@@ -1857,16 +1857,16 @@
         <v>10</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N22" s="3" t="s">
         <v>14</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="P22" s="3" t="s">
         <v>12</v>
@@ -1875,7 +1875,7 @@
         <v>15</v>
       </c>
       <c r="R22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.4">
@@ -1883,25 +1883,25 @@
         <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>11</v>
@@ -1913,16 +1913,16 @@
         <v>10</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N23" s="3" t="s">
         <v>14</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="P23" s="3" t="s">
         <v>12</v>
@@ -1931,7 +1931,7 @@
         <v>15</v>
       </c>
       <c r="R23" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.4">
@@ -1939,25 +1939,25 @@
         <v>9</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I24" s="3" t="s">
         <v>11</v>
@@ -1969,16 +1969,16 @@
         <v>10</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>14</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="P24" s="3" t="s">
         <v>12</v>
@@ -1987,7 +1987,7 @@
         <v>15</v>
       </c>
       <c r="R24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.4">
@@ -1995,25 +1995,25 @@
         <v>9</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>11</v>
@@ -2025,10 +2025,10 @@
         <v>10</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N25" s="3" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
renaming files, restoring unfinished B_covar runs, running model probs, general B_covar post processing
</commit_message>
<xml_diff>
--- a/analyses_log.xlsx
+++ b/analyses_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoesLabAdmin\Documents\BDNN_Arielli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8616842C-FEE1-4D76-999A-FF0AD8D9C8DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3347825-0F55-4406-98BE-C04515BF432C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="334" yWindow="1671" windowWidth="16372" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
+    <workbookView xWindow="15334" yWindow="866" windowWidth="16372" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="81">
   <si>
     <t>Sampling Algorithm</t>
   </si>
@@ -259,12 +259,6 @@
     <t>*All Models use a Time Variable Poisson Process (TPP) to model Preservation, except for CoVar RJMCMC HPP, which uses a Homogenous Poisson Process</t>
   </si>
   <si>
-    <t>mcmc_predictors/B_covar_rjmcmc &amp; B_covar_rjmcmc_no_translate</t>
-  </si>
-  <si>
-    <t>mcmc_predictors/B_covar_rjmcmc_hpp</t>
-  </si>
-  <si>
     <t>If 2 directories are indicated (by an "&amp;"), these are the same models w/ one difference in hyperparameter</t>
   </si>
   <si>
@@ -284,6 +278,18 @@
   </si>
   <si>
     <t>mcmc_fixshift_no_predictors/D_bdnn &amp; D_bdnn_update</t>
+  </si>
+  <si>
+    <t>mcmc_fixshift_predictors/D_mcmc</t>
+  </si>
+  <si>
+    <t>mcmc_predictors/B_covar_rjmcmc</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>mcmc_predictors/B_covar_rjmcmc_hpp_notranslate</t>
   </si>
 </sst>
 </file>
@@ -724,7 +730,7 @@
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.4"/>
@@ -928,6 +934,9 @@
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="B4" s="3" t="s">
         <v>55</v>
       </c>
@@ -970,8 +979,8 @@
       <c r="O4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="7" t="s">
-        <v>58</v>
+      <c r="P4" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>12</v>
@@ -1038,7 +1047,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>21</v>
@@ -1086,15 +1095,15 @@
         <v>14</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:19" ht="12.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>68</v>
@@ -1142,7 +1151,7 @@
         <v>14</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="R7" s="3" t="s">
         <v>14</v>
@@ -1203,7 +1212,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>18</v>
@@ -1259,7 +1268,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
@@ -1318,7 +1327,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>19</v>
@@ -1377,7 +1386,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>19</v>
@@ -1648,7 +1657,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>9</v>
@@ -1704,7 +1713,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>9</v>
@@ -1760,7 +1769,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
@@ -1816,7 +1825,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>9</v>
@@ -1925,7 +1934,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>9</v>
@@ -2329,7 +2338,7 @@
     </row>
     <row r="30" spans="1:19" ht="102.9" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
rtt plot axes work
</commit_message>
<xml_diff>
--- a/analyses_log.xlsx
+++ b/analyses_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoesLabAdmin\Documents\BDNN_Arielli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3347825-0F55-4406-98BE-C04515BF432C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436DF9A6-6D45-4810-97AE-F60E6459EFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15334" yWindow="866" windowWidth="16372" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
   </bookViews>
@@ -730,7 +730,7 @@
   <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
ltt graphs code, adding model probs
</commit_message>
<xml_diff>
--- a/analyses_log.xlsx
+++ b/analyses_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoesLabAdmin\Documents\BDNN_Arielli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436DF9A6-6D45-4810-97AE-F60E6459EFF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6491623-3BE9-4AC1-8082-C3FB503E8E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15334" yWindow="866" windowWidth="16372" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="83">
   <si>
     <t>Sampling Algorithm</t>
   </si>
@@ -223,9 +223,6 @@
     <t>Compare with 1 Myr BDMCMC, no preds, and CoVar RJMCMC</t>
   </si>
   <si>
-    <t>Tem Only</t>
-  </si>
-  <si>
     <t>Name in Files</t>
   </si>
   <si>
@@ -290,6 +287,15 @@
   </si>
   <si>
     <t>mcmc_predictors/B_covar_rjmcmc_hpp_notranslate</t>
+  </si>
+  <si>
+    <t>mcmc_predictors/B_covar_mcmc</t>
+  </si>
+  <si>
+    <t>Rep Only</t>
+  </si>
+  <si>
+    <t>Tem and Rep Only</t>
   </si>
 </sst>
 </file>
@@ -729,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EA881A-93D2-4F0C-B578-B509C4BBF0BD}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24:P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.4"/>
@@ -758,7 +764,7 @@
   <sheetData>
     <row r="1" spans="1:19" s="9" customFormat="1" ht="25.75" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>45</v>
@@ -817,7 +823,7 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>17</v>
@@ -876,7 +882,7 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
@@ -935,7 +941,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>55</v>
@@ -991,7 +997,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>55</v>
@@ -1047,7 +1053,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>21</v>
@@ -1095,7 +1101,7 @@
         <v>14</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>14</v>
@@ -1103,10 +1109,10 @@
     </row>
     <row r="7" spans="1:19" ht="12.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>30</v>
@@ -1151,13 +1157,16 @@
         <v>14</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A8" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1201,7 +1210,7 @@
         <v>14</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>12</v>
@@ -1212,7 +1221,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>18</v>
@@ -1268,7 +1277,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
@@ -1327,7 +1336,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>19</v>
@@ -1386,7 +1395,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>19</v>
@@ -1657,7 +1666,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>9</v>
@@ -1713,7 +1722,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>9</v>
@@ -1769,7 +1778,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
@@ -1825,7 +1834,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>9</v>
@@ -1934,7 +1943,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>9</v>
@@ -1990,7 +1999,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>9</v>
@@ -2049,7 +2058,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>9</v>
@@ -2094,7 +2103,7 @@
         <v>14</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>12</v>
@@ -2108,7 +2117,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>9</v>
@@ -2153,7 +2162,7 @@
         <v>14</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="Q25" s="3" t="s">
         <v>12</v>
@@ -2167,7 +2176,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>9</v>
@@ -2212,7 +2221,7 @@
         <v>14</v>
       </c>
       <c r="P26" s="7" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="Q26" s="3" t="s">
         <v>12</v>
@@ -2226,7 +2235,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>9</v>
@@ -2271,7 +2280,7 @@
         <v>14</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="Q27" s="3" t="s">
         <v>12</v>
@@ -2338,10 +2347,10 @@
     </row>
     <row r="30" spans="1:19" ht="102.9" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
b_covar post processing.  a lot of re-runs, deletions, graphing, restoration, combining logs, etc.
</commit_message>
<xml_diff>
--- a/analyses_log.xlsx
+++ b/analyses_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoesLabAdmin\Documents\BDNN_Arielli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6491623-3BE9-4AC1-8082-C3FB503E8E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BEEDC1-3295-4291-BE3E-11E9172F87E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15334" yWindow="866" windowWidth="16372" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="table" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">table!$B$1:$T$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">table!$B$1:$B$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="80">
   <si>
     <t>Sampling Algorithm</t>
   </si>
@@ -250,9 +250,6 @@
     <t>mcmc_predictors/B_bdnn_stdscaled_cbrt</t>
   </si>
   <si>
-    <t>CoVar RJMCMC *HPP</t>
-  </si>
-  <si>
     <t>*All Models use a Time Variable Poisson Process (TPP) to model Preservation, except for CoVar RJMCMC HPP, which uses a Homogenous Poisson Process</t>
   </si>
   <si>
@@ -286,13 +283,7 @@
     <t>Good</t>
   </si>
   <si>
-    <t>mcmc_predictors/B_covar_rjmcmc_hpp_notranslate</t>
-  </si>
-  <si>
     <t>mcmc_predictors/B_covar_mcmc</t>
-  </si>
-  <si>
-    <t>Rep Only</t>
   </si>
   <si>
     <t>Tem and Rep Only</t>
@@ -733,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EA881A-93D2-4F0C-B578-B509C4BBF0BD}">
-  <dimension ref="A1:S30"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24:P27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.4"/>
@@ -941,7 +932,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>55</v>
@@ -1053,7 +1044,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>21</v>
@@ -1101,24 +1092,24 @@
         <v>14</v>
       </c>
       <c r="Q6" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A7" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="R6" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="12.45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="B7" s="3" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>18</v>
@@ -1153,25 +1144,25 @@
       <c r="O7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P7" s="3" t="s">
-        <v>14</v>
+      <c r="P7" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>55</v>
@@ -1209,8 +1200,8 @@
       <c r="O8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P8" s="7" t="s">
-        <v>81</v>
+      <c r="P8" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>12</v>
@@ -1221,10 +1212,10 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>31</v>
@@ -1233,16 +1224,16 @@
         <v>55</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>38</v>
@@ -1272,12 +1263,15 @@
         <v>12</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
@@ -1292,7 +1286,7 @@
         <v>19</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>26</v>
@@ -1328,7 +1322,7 @@
         <v>12</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="S10" s="3" t="s">
         <v>28</v>
@@ -1336,7 +1330,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>19</v>
@@ -1351,7 +1345,7 @@
         <v>19</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>26</v>
@@ -1393,63 +1387,57 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A12" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="3" t="s">
+    <row r="12" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="C12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="F12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L12" s="3">
-        <v>10</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>28</v>
+      <c r="J12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L12" s="4">
+        <v>10</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.4">
@@ -1466,7 +1454,7 @@
         <v>19</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>26</v>
@@ -1519,13 +1507,13 @@
         <v>19</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>26</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>38</v>
@@ -1572,7 +1560,7 @@
         <v>19</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>26</v>
@@ -1611,56 +1599,59 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I16" s="4" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A16" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L16" s="4">
-        <v>10</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="O16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="P16" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="R16" s="4" t="s">
+      <c r="J16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="3">
+        <v>10</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R16" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1690,7 +1681,7 @@
         <v>49</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>11</v>
@@ -1746,7 +1737,7 @@
         <v>49</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>11</v>
@@ -1802,7 +1793,7 @@
         <v>49</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>11</v>
@@ -1833,9 +1824,6 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A20" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="B20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1852,13 +1840,13 @@
         <v>39</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>11</v>
@@ -1878,8 +1866,8 @@
       <c r="O20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P20" s="3" t="s">
-        <v>14</v>
+      <c r="P20" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="Q20" s="3" t="s">
         <v>12</v>
@@ -1889,6 +1877,9 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A21" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
@@ -1905,13 +1896,13 @@
         <v>39</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>39</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>11</v>
@@ -1931,8 +1922,8 @@
       <c r="O21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P21" s="7" t="s">
-        <v>15</v>
+      <c r="P21" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="Q21" s="3" t="s">
         <v>12</v>
@@ -1943,13 +1934,13 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>55</v>
@@ -1996,10 +1987,13 @@
       <c r="R22" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="S22" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>9</v>
@@ -2017,13 +2011,13 @@
         <v>39</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>11</v>
@@ -2043,8 +2037,8 @@
       <c r="O23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P23" s="3" t="s">
-        <v>14</v>
+      <c r="P23" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>12</v>
@@ -2058,7 +2052,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>9</v>
@@ -2082,7 +2076,7 @@
         <v>50</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>11</v>
@@ -2103,7 +2097,7 @@
         <v>14</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>12</v>
@@ -2117,7 +2111,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>9</v>
@@ -2141,7 +2135,7 @@
         <v>50</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>11</v>
@@ -2162,7 +2156,7 @@
         <v>14</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q25" s="3" t="s">
         <v>12</v>
@@ -2176,7 +2170,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>9</v>
@@ -2200,7 +2194,7 @@
         <v>50</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J26" s="3" t="s">
         <v>11</v>
@@ -2221,7 +2215,7 @@
         <v>14</v>
       </c>
       <c r="P26" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q26" s="3" t="s">
         <v>12</v>
@@ -2234,9 +2228,6 @@
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A27" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
@@ -2253,13 +2244,13 @@
         <v>39</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>11</v>
@@ -2280,7 +2271,7 @@
         <v>14</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="Q27" s="3" t="s">
         <v>12</v>
@@ -2288,77 +2279,17 @@
       <c r="R27" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="S27" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="B28" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L28" s="3">
-        <v>10</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="P28" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="R28" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" ht="102.9" x14ac:dyDescent="0.4">
-      <c r="A30" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30" s="8" t="s">
+    </row>
+    <row r="29" spans="1:19" ht="102.9" x14ac:dyDescent="0.4">
+      <c r="A29" s="2" t="s">
         <v>68</v>
       </c>
+      <c r="B29" s="8" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:T1" xr:uid="{A9EA881A-93D2-4F0C-B578-B509C4BBF0BD}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:T22">
-      <sortCondition descending="1" ref="B1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="B1:B29" xr:uid="{A9EA881A-93D2-4F0C-B578-B509C4BBF0BD}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
MBD runs, LTT graphs, making sure things are complete and restoring if needed
</commit_message>
<xml_diff>
--- a/analyses_log.xlsx
+++ b/analyses_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoesLabAdmin\Documents\BDNN_Arielli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BEEDC1-3295-4291-BE3E-11E9172F87E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6D6307-18BA-44A8-84ED-19C35A4FE7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15334" yWindow="866" windowWidth="16372" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="80">
   <si>
     <t>Sampling Algorithm</t>
   </si>
@@ -232,9 +232,6 @@
     <t>mcmc_no_predictors/RJMCMC</t>
   </si>
   <si>
-    <t>mcmc_no_predictors/A_bdnn_update &amp; A_bdnn</t>
-  </si>
-  <si>
     <t>mcmc_no_predictors/A_mcmc</t>
   </si>
   <si>
@@ -250,9 +247,6 @@
     <t>mcmc_predictors/B_bdnn_stdscaled_cbrt</t>
   </si>
   <si>
-    <t>*All Models use a Time Variable Poisson Process (TPP) to model Preservation, except for CoVar RJMCMC HPP, which uses a Homogenous Poisson Process</t>
-  </si>
-  <si>
     <t>If 2 directories are indicated (by an "&amp;"), these are the same models w/ one difference in hyperparameter</t>
   </si>
   <si>
@@ -287,6 +281,12 @@
   </si>
   <si>
     <t>Tem and Rep Only</t>
+  </si>
+  <si>
+    <t>*All Models use a Time Variable Poisson Process (TPP) to model Preservation</t>
+  </si>
+  <si>
+    <t>mcmc_no_predictors/A_bdnn_update &amp; A_bdnn*</t>
   </si>
 </sst>
 </file>
@@ -727,7 +727,7 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.4"/>
@@ -932,7 +932,7 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>55</v>
@@ -988,7 +988,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>55</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>21</v>
@@ -1092,7 +1092,7 @@
         <v>14</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>14</v>
@@ -1100,7 +1100,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>18</v>
@@ -1144,19 +1144,22 @@
       <c r="O7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P7" s="7" t="s">
-        <v>79</v>
+      <c r="P7" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="R7" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>18</v>
@@ -1212,7 +1215,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>19</v>
@@ -1271,7 +1274,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
@@ -1330,7 +1333,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>19</v>
@@ -1388,6 +1391,9 @@
       </c>
     </row>
     <row r="12" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
@@ -1441,6 +1447,9 @@
       </c>
     </row>
     <row r="13" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="B13" s="4" t="s">
         <v>19</v>
       </c>
@@ -1494,6 +1503,9 @@
       </c>
     </row>
     <row r="14" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="B14" s="4" t="s">
         <v>19</v>
       </c>
@@ -1533,8 +1545,8 @@
       <c r="N14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="O14" s="6" t="s">
-        <v>15</v>
+      <c r="O14" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="P14" s="4" t="s">
         <v>15</v>
@@ -1547,6 +1559,9 @@
       </c>
     </row>
     <row r="15" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1586,8 +1601,8 @@
       <c r="N15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="O15" s="6" t="s">
-        <v>15</v>
+      <c r="O15" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="P15" s="4" t="s">
         <v>15</v>
@@ -1601,7 +1616,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>9</v>
@@ -1657,7 +1672,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>9</v>
@@ -1713,7 +1728,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>9</v>
@@ -1769,7 +1784,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
@@ -1878,7 +1893,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>9</v>
@@ -1934,7 +1949,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>9</v>
@@ -1993,7 +2008,7 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>9</v>
@@ -2038,7 +2053,7 @@
         <v>14</v>
       </c>
       <c r="P23" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q23" s="3" t="s">
         <v>12</v>
@@ -2052,7 +2067,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>9</v>
@@ -2097,7 +2112,7 @@
         <v>14</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q24" s="3" t="s">
         <v>12</v>
@@ -2111,7 +2126,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>9</v>
@@ -2156,7 +2171,7 @@
         <v>14</v>
       </c>
       <c r="P25" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q25" s="3" t="s">
         <v>12</v>
@@ -2170,7 +2185,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>9</v>
@@ -2215,7 +2230,7 @@
         <v>14</v>
       </c>
       <c r="P26" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="Q26" s="3" t="s">
         <v>12</v>
@@ -2280,12 +2295,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="102.9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:19" ht="51.45" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
getting unique country codes list + correct bdmcmc run test + rerun of nb + newly labelled occurrences graph
</commit_message>
<xml_diff>
--- a/analyses_log.xlsx
+++ b/analyses_log.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoesLabAdmin\Documents\BDNN_Arielli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F997B3A4-5B22-45E9-85B0-8921AB0F2B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A22EC4-E405-4D4E-A2C5-EBDA91AB8363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="386" yWindow="1200" windowWidth="20665" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
+    <workbookView xWindow="-729" yWindow="1569" windowWidth="29263" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">table!$B$1:$B$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">table!$B$1:$B$32</definedName>
     <definedName name="HighlightRow">13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="87">
   <si>
     <t>Sampling Algorithm</t>
   </si>
@@ -293,9 +293,6 @@
     <t>mcmc_predictors/B_bdnn_lats_only</t>
   </si>
   <si>
-    <t>Varies</t>
-  </si>
-  <si>
     <t>Tem reps 4, 7, 9 poor diagnostics</t>
   </si>
   <si>
@@ -303,6 +300,15 @@
   </si>
   <si>
     <t>Diagnostics varied by replicate</t>
+  </si>
+  <si>
+    <t>200 mi</t>
+  </si>
+  <si>
+    <t>Poor</t>
+  </si>
+  <si>
+    <t>MCMC + TI</t>
   </si>
 </sst>
 </file>
@@ -339,12 +345,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -359,19 +371,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -743,11 +761,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EA881A-93D2-4F0C-B578-B509C4BBF0BD}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:S29"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E13" sqref="E13"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.4"/>
@@ -832,77 +850,26 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="1">
-        <v>10</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A3" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>46</v>
@@ -941,27 +908,27 @@
         <v>14</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>46</v>
@@ -988,7 +955,7 @@
         <v>10</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>33</v>
+        <v>84</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>32</v>
@@ -1000,21 +967,24 @@
         <v>14</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>55</v>
@@ -1052,46 +1022,43 @@
       <c r="O5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="3" t="s">
-        <v>15</v>
+      <c r="P5" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>81</v>
+        <v>12</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>39</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>11</v>
@@ -1111,155 +1078,61 @@
       <c r="O6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>14</v>
+      <c r="P6" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A7" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="B8" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="1">
-        <v>10</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="1">
-        <v>10</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="P8" s="3"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>38</v>
@@ -1286,39 +1159,36 @@
         <v>14</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>38</v>
@@ -1345,7 +1215,7 @@
         <v>14</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>15</v>
@@ -1359,7 +1229,7 @@
         <v>67</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>31</v>
@@ -1368,16 +1238,16 @@
         <v>55</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>38</v>
@@ -1409,19 +1279,16 @@
       <c r="R11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S11" s="1" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>55</v>
@@ -1430,7 +1297,7 @@
         <v>19</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>26</v>
@@ -1459,25 +1326,28 @@
       <c r="O12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P12" s="3" t="s">
-        <v>15</v>
+      <c r="P12" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>55</v>
@@ -1486,7 +1356,7 @@
         <v>19</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>26</v>
@@ -1515,8 +1385,8 @@
       <c r="O13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P13" s="3" t="s">
-        <v>15</v>
+      <c r="P13" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="Q13" s="1" t="s">
         <v>12</v>
@@ -1524,16 +1394,19 @@
       <c r="R13" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="S13" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>55</v>
@@ -1542,13 +1415,13 @@
         <v>19</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>38</v>
@@ -1579,6 +1452,9 @@
       </c>
       <c r="R14" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.4">
@@ -1598,13 +1474,13 @@
         <v>19</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>38</v>
@@ -1627,8 +1503,8 @@
       <c r="O15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P15" s="1" t="s">
-        <v>14</v>
+      <c r="P15" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>12</v>
@@ -1639,25 +1515,25 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>49</v>
@@ -1683,8 +1559,8 @@
       <c r="O16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P16" s="1" t="s">
-        <v>14</v>
+      <c r="P16" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>12</v>
@@ -1695,31 +1571,31 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>11</v>
@@ -1751,31 +1627,31 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>11</v>
@@ -1807,7 +1683,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
@@ -1831,7 +1707,7 @@
         <v>49</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>11</v>
@@ -1862,6 +1738,9 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A20" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="B20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1878,13 +1757,13 @@
         <v>39</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>11</v>
@@ -1904,8 +1783,8 @@
       <c r="O20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P20" s="3" t="s">
-        <v>15</v>
+      <c r="P20" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="Q20" s="1" t="s">
         <v>12</v>
@@ -1916,7 +1795,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>9</v>
@@ -1934,13 +1813,13 @@
         <v>39</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>11</v>
@@ -1972,13 +1851,13 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>55</v>
@@ -1990,13 +1869,13 @@
         <v>39</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>11</v>
@@ -2025,19 +1904,13 @@
       <c r="R22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S22" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A23" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>55</v>
@@ -2049,13 +1922,13 @@
         <v>39</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>11</v>
@@ -2076,7 +1949,7 @@
         <v>14</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>12</v>
@@ -2084,19 +1957,16 @@
       <c r="R23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S23" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>55</v>
@@ -2108,13 +1978,13 @@
         <v>39</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>11</v>
@@ -2134,8 +2004,8 @@
       <c r="O24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P24" s="3" t="s">
-        <v>77</v>
+      <c r="P24" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>12</v>
@@ -2143,13 +2013,10 @@
       <c r="R24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S24" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>9</v>
@@ -2167,13 +2034,13 @@
         <v>39</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>11</v>
@@ -2193,8 +2060,8 @@
       <c r="O25" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P25" s="3" t="s">
-        <v>77</v>
+      <c r="P25" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>12</v>
@@ -2208,7 +2075,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>9</v>
@@ -2232,7 +2099,7 @@
         <v>50</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>11</v>
@@ -2267,7 +2134,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>9</v>
@@ -2285,13 +2152,13 @@
         <v>39</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>11</v>
@@ -2311,46 +2178,223 @@
       <c r="O27" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P27" s="1" t="s">
-        <v>14</v>
+      <c r="P27" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="Q27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L28" s="1">
+        <v>10</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L29" s="1">
+        <v>10</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L30" s="1">
+        <v>10</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S30" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="R27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" ht="51.45" x14ac:dyDescent="0.4">
-      <c r="A29" s="2" t="s">
+    </row>
+    <row r="32" spans="1:19" ht="51.45" x14ac:dyDescent="0.4">
+      <c r="A32" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>78</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B29" xr:uid="{A9EA881A-93D2-4F0C-B578-B509C4BBF0BD}"/>
+  <autoFilter ref="B1:B32" xr:uid="{A9EA881A-93D2-4F0C-B578-B509C4BBF0BD}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A4:XFD4">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:S29">
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="A1:S32">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>"row()=cell(""row"")"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>ROW(A1)=HighlightRow</formula>
+    </cfRule>
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>"row()=cell(""row"")"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>ROW(A1)=HighlightRow</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A5:XFD5">
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>ROW()=CELL("row")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
proper renaming of sub directories, edit of A_mcmc_syn for resub
</commit_message>
<xml_diff>
--- a/analyses_log.xlsx
+++ b/analyses_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoesLabAdmin\Documents\BDNN_Arielli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A22EC4-E405-4D4E-A2C5-EBDA91AB8363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D3A203-9F4C-4E44-8346-2F7505C2DF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-729" yWindow="1569" windowWidth="29263" windowHeight="16020" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
+    <workbookView xWindow="3386" yWindow="1843" windowWidth="23700" windowHeight="15986" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="86">
   <si>
     <t>Sampling Algorithm</t>
   </si>
@@ -233,9 +233,6 @@
     <t>mcmc_no_predictors/RJMCMC</t>
   </si>
   <si>
-    <t>mcmc_no_predictors/A_mcmc</t>
-  </si>
-  <si>
     <t>mcmc_predictors/B_bdnn_stdscaled_only</t>
   </si>
   <si>
@@ -293,9 +290,6 @@
     <t>mcmc_predictors/B_bdnn_lats_only</t>
   </si>
   <si>
-    <t>Tem reps 4, 7, 9 poor diagnostics</t>
-  </si>
-  <si>
     <t>Mixed</t>
   </si>
   <si>
@@ -309,6 +303,9 @@
   </si>
   <si>
     <t>MCMC + TI</t>
+  </si>
+  <si>
+    <t>mcmc_no_predictors/A_mcmc_200_iterations</t>
   </si>
 </sst>
 </file>
@@ -764,8 +761,8 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J3" sqref="J3"/>
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.4"/>
@@ -908,7 +905,7 @@
         <v>14</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>15</v>
@@ -955,7 +952,7 @@
         <v>10</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>32</v>
@@ -967,7 +964,7 @@
         <v>14</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>15</v>
@@ -978,7 +975,7 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>55</v>
@@ -1034,7 +1031,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>55</v>
@@ -1070,7 +1067,7 @@
         <v>10</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>33</v>
+        <v>82</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>32</v>
@@ -1078,22 +1075,19 @@
       <c r="O6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="3" t="s">
-        <v>15</v>
+      <c r="P6" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="R6" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B7" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>31</v>
@@ -1102,7 +1096,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>30</v>
@@ -1111,7 +1105,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
@@ -1159,7 +1153,7 @@
         <v>14</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R9" s="1" t="s">
         <v>14</v>
@@ -1167,7 +1161,7 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>18</v>
@@ -1215,7 +1209,7 @@
         <v>14</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="R10" s="1" t="s">
         <v>15</v>
@@ -1226,7 +1220,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>18</v>
@@ -1282,7 +1276,7 @@
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>19</v>
@@ -1341,7 +1335,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>19</v>
@@ -1400,7 +1394,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>19</v>
@@ -1459,7 +1453,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>19</v>
@@ -1515,7 +1509,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>19</v>
@@ -1571,7 +1565,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>19</v>
@@ -1627,7 +1621,7 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>19</v>
@@ -1683,7 +1677,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>9</v>
@@ -1739,7 +1733,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>9</v>
@@ -1795,7 +1789,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>9</v>
@@ -1851,7 +1845,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>9</v>
@@ -1960,7 +1954,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>9</v>
@@ -2016,7 +2010,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>9</v>
@@ -2075,7 +2069,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>9</v>
@@ -2120,7 +2114,7 @@
         <v>14</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q26" s="1" t="s">
         <v>12</v>
@@ -2134,7 +2128,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>9</v>
@@ -2179,7 +2173,7 @@
         <v>14</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>12</v>
@@ -2193,7 +2187,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>9</v>
@@ -2238,7 +2232,7 @@
         <v>14</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q28" s="1" t="s">
         <v>12</v>
@@ -2252,7 +2246,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>9</v>
@@ -2297,7 +2291,7 @@
         <v>14</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>12</v>
@@ -2311,7 +2305,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>9</v>
@@ -2359,21 +2353,21 @@
         <v>14</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="R30" s="1" t="s">
         <v>15</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="51.45" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
starting mbd runs 1 myr temp C_covar, rerun of eda to output spatial occs graphs by rep, syn, tem, and all taxa age range plot
</commit_message>
<xml_diff>
--- a/analyses_log.xlsx
+++ b/analyses_log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SimoesLabAdmin\Documents\BDNN_Arielli\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D3A203-9F4C-4E44-8346-2F7505C2DF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D06806-62AE-437A-ACEB-C4540804353E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3386" yWindow="1843" windowWidth="23700" windowHeight="15986" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
+    <workbookView xWindow="3386" yWindow="1809" windowWidth="23700" windowHeight="15985" xr2:uid="{2B31D40A-C581-4DA9-854D-6A8F263900C8}"/>
   </bookViews>
   <sheets>
     <sheet name="table" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="86">
   <si>
     <t>Sampling Algorithm</t>
   </si>
@@ -302,10 +302,10 @@
     <t>Poor</t>
   </si>
   <si>
-    <t>MCMC + TI</t>
-  </si>
-  <si>
     <t>mcmc_no_predictors/A_mcmc_200_iterations</t>
+  </si>
+  <si>
+    <t>mcmc_fixshift_no_predictors/BDMCMC</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -382,17 +382,48 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -761,8 +792,8 @@
   <dimension ref="A1:S32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q25" sqref="Q25"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.4"/>
@@ -847,16 +878,67 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1">
+        <v>10</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>59</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -901,11 +983,11 @@
       <c r="O3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>14</v>
+      <c r="P3" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>15</v>
@@ -1031,7 +1113,7 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>55</v>
@@ -1075,8 +1157,8 @@
       <c r="O6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="1" t="s">
-        <v>14</v>
+      <c r="P6" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="Q6" s="1" t="s">
         <v>74</v>
@@ -1086,35 +1168,132 @@
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P7" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="1">
+        <v>10</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="B8" s="1" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="P8" s="3"/>
+      <c r="D8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="1">
+        <v>10</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>18</v>
@@ -1153,36 +1332,36 @@
         <v>14</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>55</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>38</v>
@@ -1209,69 +1388,72 @@
         <v>14</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>74</v>
+        <v>12</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="B11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="D11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L11" s="1">
-        <v>10</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q11" s="1" t="s">
+      <c r="J11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="6">
+        <v>10</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="P11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="R11" s="1" t="s">
-        <v>15</v>
+      <c r="R11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.4">
@@ -1291,7 +1473,7 @@
         <v>19</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>26</v>
@@ -1327,7 +1509,7 @@
         <v>12</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="S12" s="1" t="s">
         <v>28</v>
@@ -1356,7 +1538,7 @@
         <v>26</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>38</v>
@@ -1379,8 +1561,8 @@
       <c r="O13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P13" s="1" t="s">
-        <v>14</v>
+      <c r="P13" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="Q13" s="1" t="s">
         <v>12</v>
@@ -1392,7 +1574,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:19" ht="12.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>66</v>
       </c>
@@ -1415,7 +1597,7 @@
         <v>26</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>38</v>
@@ -1438,8 +1620,8 @@
       <c r="O14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P14" s="1" t="s">
-        <v>14</v>
+      <c r="P14" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>12</v>
@@ -1497,8 +1679,8 @@
       <c r="O15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P15" s="3" t="s">
-        <v>15</v>
+      <c r="P15" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>12</v>
@@ -1553,8 +1735,8 @@
       <c r="O16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P16" s="3" t="s">
-        <v>15</v>
+      <c r="P16" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>12</v>
@@ -2373,24 +2555,6 @@
   </sheetData>
   <autoFilter ref="B1:B32" xr:uid="{A9EA881A-93D2-4F0C-B578-B509C4BBF0BD}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A1:S32">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>"row()=cell(""row"")"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>ROW(A1)=HighlightRow</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>"row()=cell(""row"")"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A5:XFD5">
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>ROW()=CELL("row")</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>